<commit_message>
Add traffic control problem
</commit_message>
<xml_diff>
--- a/newData.xlsx
+++ b/newData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\SS1\src\main\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5412FAF9-74AD-4D4D-8E54-EFCD5213B426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BB240E7-FC45-4B91-A403-0DA49A735686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5865" yWindow="-14025" windowWidth="20010" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>Col 1</t>
   </si>
@@ -178,17 +178,23 @@
     <t>User Input</t>
   </si>
   <si>
-    <t>1,2,2,1</t>
+    <t>0.622</t>
   </si>
   <si>
-    <t>3,1,1,2</t>
+    <t>0.1266</t>
+  </si>
+  <si>
+    <t>0.138983</t>
+  </si>
+  <si>
+    <t>0.172666</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,8 +244,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +297,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -559,16 +583,31 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -853,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CG221"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1159,7 +1198,7 @@
       </c>
     </row>
     <row r="16" spans="1:31" ht="26.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="49" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="31"/>
@@ -1195,10 +1234,10 @@
     </row>
     <row r="17" spans="1:85">
       <c r="A17" s="43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" s="43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -1232,10 +1271,10 @@
     </row>
     <row r="18" spans="1:85">
       <c r="A18" s="43">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B18" s="43">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
@@ -1269,10 +1308,10 @@
     </row>
     <row r="19" spans="1:85">
       <c r="A19" s="44">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B19" s="44">
-        <v>5386</v>
+        <v>0</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
@@ -1306,10 +1345,10 @@
     </row>
     <row r="20" spans="1:85">
       <c r="A20" s="45">
-        <v>3</v>
+        <v>1</v>
       </c>
-      <c r="B20" s="45">
-        <v>5</v>
+      <c r="B20" s="46">
+        <v>2</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
@@ -1396,21 +1435,15 @@
       <c r="CG20" s="31"/>
     </row>
     <row r="21" spans="1:85">
-      <c r="A21" s="45">
-        <v>11111</v>
+      <c r="A21" s="48">
+        <v>1</v>
       </c>
-      <c r="B21" s="50">
-        <v>22222</v>
+      <c r="B21" s="46" t="s">
+        <v>47</v>
       </c>
-      <c r="C21" s="46">
-        <v>33333</v>
-      </c>
-      <c r="D21" s="46">
-        <v>44444</v>
-      </c>
-      <c r="E21" s="46">
-        <v>55555</v>
-      </c>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="31"/>
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
@@ -1493,39 +1526,31 @@
       <c r="CG21" s="31"/>
     </row>
     <row r="22" spans="1:85">
-      <c r="A22" s="48">
-        <v>2</v>
+      <c r="A22" s="53">
+        <v>3</v>
       </c>
-      <c r="B22" s="47">
-        <v>1062016</v>
+      <c r="B22" s="54" t="s">
+        <v>48</v>
       </c>
       <c r="C22" s="47">
-        <v>31052017</v>
+        <v>1600</v>
       </c>
-      <c r="D22" s="47">
-        <v>10720</v>
+      <c r="D22" s="55" t="s">
+        <v>49</v>
       </c>
-      <c r="E22" s="47">
-        <v>12800</v>
+      <c r="E22" s="51">
+        <v>1680</v>
       </c>
-      <c r="F22" s="47">
-        <v>10</v>
+      <c r="F22" s="56" t="s">
+        <v>50</v>
       </c>
-      <c r="G22" s="36">
-        <v>1062016</v>
+      <c r="G22" s="52">
+        <v>1714</v>
       </c>
-      <c r="H22" s="36">
-        <v>31052017</v>
-      </c>
-      <c r="I22" s="36">
-        <v>14800</v>
-      </c>
-      <c r="J22" s="36">
-        <v>17400</v>
-      </c>
-      <c r="K22" s="36">
-        <v>10</v>
-      </c>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
       <c r="L22" s="31"/>
       <c r="M22" s="31"/>
       <c r="N22" s="31"/>
@@ -1602,37 +1627,17 @@
       <c r="CG22" s="31"/>
     </row>
     <row r="23" spans="1:85">
-      <c r="A23" s="49">
-        <v>2</v>
-      </c>
-      <c r="B23" s="47">
-        <v>1062016</v>
-      </c>
-      <c r="C23" s="47">
-        <v>31052017</v>
-      </c>
-      <c r="D23" s="47">
-        <v>10880</v>
-      </c>
-      <c r="E23" s="47">
-        <v>12960</v>
-      </c>
-      <c r="F23" s="47">
-        <v>9</v>
-      </c>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36">
-        <v>31052017</v>
-      </c>
-      <c r="I23" s="36">
-        <v>1500</v>
-      </c>
-      <c r="J23" s="36">
-        <v>17600</v>
-      </c>
-      <c r="K23" s="36">
-        <v>9</v>
-      </c>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
       <c r="L23" s="31"/>
       <c r="M23" s="31"/>
       <c r="N23" s="31"/>
@@ -1709,39 +1714,17 @@
       <c r="CG23" s="31"/>
     </row>
     <row r="24" spans="1:85">
-      <c r="A24" s="49">
-        <v>2</v>
-      </c>
-      <c r="B24" s="47">
-        <v>1012017</v>
-      </c>
-      <c r="C24" s="47">
-        <v>31122017</v>
-      </c>
-      <c r="D24" s="47">
-        <v>11040</v>
-      </c>
-      <c r="E24" s="47">
-        <v>12960</v>
-      </c>
-      <c r="F24" s="47">
-        <v>10</v>
-      </c>
-      <c r="G24" s="36">
-        <v>1012017</v>
-      </c>
-      <c r="H24" s="36">
-        <v>31122017</v>
-      </c>
-      <c r="I24" s="36">
-        <v>15200</v>
-      </c>
-      <c r="J24" s="36">
-        <v>17600</v>
-      </c>
-      <c r="K24" s="36">
-        <v>10</v>
-      </c>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
       <c r="L24" s="31"/>
       <c r="M24" s="31"/>
       <c r="N24" s="31"/>
@@ -1817,13 +1800,9 @@
       <c r="CF24" s="31"/>
       <c r="CG24" s="31"/>
     </row>
-    <row r="25" spans="1:85">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
+    <row r="25" spans="1:85" ht="21" customHeight="1">
+      <c r="A25" s="50"/>
+      <c r="B25" s="50"/>
       <c r="AF25" s="31"/>
       <c r="AG25" s="31"/>
       <c r="AH25" s="31"/>

</xml_diff>